<commit_message>
working on ai_model - visualise data
</commit_message>
<xml_diff>
--- a/dnabot/MRes2024/transformation/results/results_serial_dilution_Team1_Serial_Dilution.xlsx
+++ b/dnabot/MRes2024/transformation/results/results_serial_dilution_Team1_Serial_Dilution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baldwin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\projectPro-Ubuntu-22.04\home\vmuser\projectpro\s5fork\dnabot\dnabot\MRes2024\transformation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{61596CA2-9CB8-46DB-BB4D-761F64B85F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C0D61DB-2C3F-4ADA-B73A-E86D524A57A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6758EE-45B0-42CE-B3BE-4FF85063B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{911C6152-1B23-48A7-B8BA-37BD02AEC135}"/>
+    <workbookView xWindow="2910" yWindow="-13980" windowWidth="21600" windowHeight="11100" xr2:uid="{911C6152-1B23-48A7-B8BA-37BD02AEC135}"/>
   </bookViews>
   <sheets>
     <sheet name="End point -End point" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,9 +361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,7 +401,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -507,7 +507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,63 +659,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8B503D-FD72-49DD-96B1-FAAC21C83883}">
   <dimension ref="A3:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>1</v>
       </c>
@@ -756,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -796,7 +796,7 @@
       <c r="M16" s="5"/>
       <c r="O16" s="14"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -835,7 +835,7 @@
       </c>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -913,7 +913,7 @@
       </c>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -991,7 +991,7 @@
       </c>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="M23" s="11"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>335.85714285714283</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>8.3152184062029981</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1216,12 +1216,12 @@
         <v>2.4758200273679707</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>1</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>3.1622776601683795</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40">
         <f>B39/B38*100</f>
         <v>1.1208789182313401</v>
@@ -1944,15 +1944,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="fdb0aa7a-bcb3-47de-829e-35c168fa1879" xsi:nil="true"/>
@@ -1963,14 +1954,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C3A4F8-F665-4E01-8F6D-B0F516D26C5A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94C3A4F8-F665-4E01-8F6D-B0F516D26C5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3937d1e2-c03a-4fc1-8763-472fa3d14f8b"/>
+    <ds:schemaRef ds:uri="fdb0aa7a-bcb3-47de-829e-35c168fa1879"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0C3CCF4-6A0E-4A39-915C-1946F2647E51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84D16F33-E80B-4437-90DB-81F4A3882134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fdb0aa7a-bcb3-47de-829e-35c168fa1879"/>
+    <ds:schemaRef ds:uri="3937d1e2-c03a-4fc1-8763-472fa3d14f8b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84D16F33-E80B-4437-90DB-81F4A3882134}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0C3CCF4-6A0E-4A39-915C-1946F2647E51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>